<commit_message>
add linux dir operation
</commit_message>
<xml_diff>
--- a/Linux学习.xlsx
+++ b/Linux学习.xlsx
@@ -5,15 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19056\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19056\Desktop\study\daily_learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B321BB9-5126-4B95-BA67-40ED165E4BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C4144D-4395-42F4-A039-0AECD90F8941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B8ADA33-6A6F-4E1C-8902-59F3CB9A88BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3B8ADA33-6A6F-4E1C-8902-59F3CB9A88BC}"/>
   </bookViews>
   <sheets>
     <sheet name="目录介绍" sheetId="1" r:id="rId1"/>
+    <sheet name="文件和目录管理" sheetId="2" r:id="rId2"/>
+    <sheet name="Linux打包（归档）和压缩" sheetId="3" r:id="rId3"/>
+    <sheet name="Vim文本编辑器" sheetId="4" r:id="rId4"/>
+    <sheet name="Linux文本处理" sheetId="5" r:id="rId5"/>
+    <sheet name="Linux软件安装" sheetId="6" r:id="rId6"/>
+    <sheet name="Linux用户和用户组管理" sheetId="7" r:id="rId7"/>
+    <sheet name="Linux权限管理" sheetId="8" r:id="rId8"/>
+    <sheet name="Linux文件系统管理" sheetId="9" r:id="rId9"/>
+    <sheet name="Linux高级文件系统管理" sheetId="10" r:id="rId10"/>
+    <sheet name="Linux系统管理" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>/home</t>
   </si>
@@ -342,12 +352,188 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t xml:space="preserve"> 目录操作命令</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cd</t>
+  </si>
+  <si>
+    <t>ls</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">mv </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF4D4D4D"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>find</t>
+  </si>
+  <si>
+    <t>rmdir</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>切换目录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">命令格式：cd 目录名
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF4F4F4F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cd /    #切换到根目录      
+cd ~    #切换到主目录      
+cd -    #切换到上次访问的目录 
+cd ..   #返回上一级目录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pwd 查看当前工作路径（绝对路径）</t>
+  </si>
+  <si>
+    <t>创建目录</t>
+  </si>
+  <si>
+    <t>mkdir</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pwd</t>
+  </si>
+  <si>
+    <t>命令格式：mkdir [-选项] 目录名
+选项： -p：递归创建目录。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看当前目录下的
+目录和文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>命令格式：rmdir 目录名 （只能删除空目录）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除目录或文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>命令格式：rm [-rf] 目录名或文件名
+选项：     -f：不提示，强制删除文件或目录；
+           -i：删除已有文件或目录之前先询问用户；
+           -r,-R：递归删除，将指定目录下的所有文件与子目录一并删除；
+           -v：显示指令的详细执行过程。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rm -rf data/    #删除当前目录下data这个目录
+rm -rf *   #删除当前目录下所有文件和目录，慎用~
+rm -rf /*  #【自杀命令！慎用！慎用！慎用！】将根目录下的所有文件全部删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+mkdir  data/    在当前目录下创建一个名为aaa的目录
+mkdir -p hadoop/data/ 在当前目录下创建hadoop一并创建子目录data
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF4D4D4D"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>命令格式：mv 旧目录名 新目录名</t>
+  </si>
+  <si>
+    <t>目录重命名/移动目录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拷贝目录或文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>命令格式：cp [-选项] 目录名称 目录拷贝的目标位置
+选项： -r：表示递归复制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cp  -r  apps/  Data/  #将apps目录复制到Data目录下</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>命令格式：find 目录 参数 文件名称或者目录名</t>
+  </si>
+  <si>
+    <t>搜索目录</t>
+  </si>
+  <si>
+    <t>find /tmp -name 'a*' 查找/tmp目录下的所有以a开头的目录或文件。</t>
+  </si>
+  <si>
+    <t>mv hadoop/ hadoop01/ #将hadoop名改为hadoop01
+mv  data  Data/     # 将data这个目录移动到Data这个目录下</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>命令格式：ls [-选项] 目录名
+选项：    -a：列出当前目录所有文件和目录
+          -l：以列表的形式显示文件和目录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文件操作命令</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -386,6 +572,83 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF4D4D4D"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF4F4F4F"/>
+      <name val="楷体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF4D4D4D"/>
+      <name val="楷体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF4D4D4D"/>
+      <name val="楷体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="楷体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF4F4F4F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF4F4F4F"/>
+      <name val="楷体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="楷体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="楷体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="17"/>
+      <color rgb="FF4F4F4F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -409,7 +672,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -427,6 +690,84 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -744,7 +1085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99BFE3A7-FC9A-4233-93DC-7A3F1E9E5E51}">
   <dimension ref="G1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
@@ -802,7 +1143,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="7:8" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="7:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="G7" s="1" t="s">
         <v>11</v>
       </c>
@@ -903,4 +1244,321 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB78517-6256-4E13-B8F3-0C3FF48F9A60}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C13E02-146F-4229-A239-87DAFA7AAD5A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61D97E5-27B0-4A91-93BA-FE4F8F923C32}">
+  <dimension ref="C1:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="7.875" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" style="30" customWidth="1"/>
+    <col min="5" max="5" width="22.875" style="28" customWidth="1"/>
+    <col min="6" max="6" width="70.875" customWidth="1"/>
+    <col min="7" max="7" width="70.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:7" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D1" s="7"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+    </row>
+    <row r="2" spans="3:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="C2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="17"/>
+    </row>
+    <row r="3" spans="3:7" ht="57" x14ac:dyDescent="0.2">
+      <c r="C3" s="12"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4" spans="3:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="12"/>
+      <c r="D4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="20"/>
+    </row>
+    <row r="5" spans="3:7" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="C5" s="12"/>
+      <c r="D5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6" spans="3:7" ht="57" x14ac:dyDescent="0.2">
+      <c r="C6" s="12"/>
+      <c r="D6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="C7" s="12"/>
+      <c r="D7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="3:7" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="C8" s="12"/>
+      <c r="D8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="23"/>
+      <c r="F8" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="C9" s="12"/>
+      <c r="D9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="C10" s="12"/>
+      <c r="D10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="C11" s="12"/>
+      <c r="D11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D12" s="29"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13" spans="3:7" ht="43.5" x14ac:dyDescent="0.2">
+      <c r="C13" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="3:7" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D14" s="29"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="3:7" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D15" s="29"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E5:F5"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B44BD4A-7367-4592-97B5-03EDBAED7504}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F8F268-C967-4E9C-BAED-BBCBB996C824}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFE0DBC-F75C-4F9C-93BE-225A71413FD8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107D198B-C0E8-4CC9-9C83-0734305E47E5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B6BA336-2E3F-433A-AA21-F42399CD5256}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{348678F1-38D5-40CB-9FBF-9259A2612466}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5CF5F26-A882-4CC5-B3AB-8F5C4C832E00}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>